<commit_message>
Adding a log file Edge 256
</commit_message>
<xml_diff>
--- a/Logfiles/AverageRTT_512.xlsx
+++ b/Logfiles/AverageRTT_512.xlsx
@@ -91,6 +91,1789 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average RTT (512</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Byte Message)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11493478087966279"/>
+          <c:y val="0.24235909619085119"/>
+          <c:w val="0.84326871072934062"/>
+          <c:h val="0.50081949458364006"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EdgeTriggered</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>4992</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5988</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6984</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7980</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8976</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9972</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10968</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11964</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12960</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13956</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14952</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15948</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16944</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17940</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18936</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19932</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20928</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21924</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22920</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23916</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>24912</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25908</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>26904</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>27900</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>28896</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>29892</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>30888</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>31884</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>32880</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>33876</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>34872</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>35868</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>36864</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>37860</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>38856</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>39852</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>40848</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>21.297000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.491</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.635000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33.926000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38.113</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.222999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>37.143999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>56.076999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>56.006999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>67.015000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>63.381999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65.974000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65.831000000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>76.001999999999995</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>108.342</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>108.276</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>104.895</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>102.94799999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>126.798</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>169.61099999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>147.13800000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>150.833</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>131.98500000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>143.899</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>159.22</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>149.958</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>182.11099999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>210.57900000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>172.51499999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>175.047</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>203.37700000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>236.59399999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>195.738</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>211.197</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>207.536</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>241.239</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>211.25899999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LevelTriggered</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>4992</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5988</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6984</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7980</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8976</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9972</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10968</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11964</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12960</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13956</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14952</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15948</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16944</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17940</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18936</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19932</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20928</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21924</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22920</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23916</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>24912</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25908</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>26904</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>27900</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>28896</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>29892</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>30888</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>31884</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>32880</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>33876</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>34872</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>35868</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>36864</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>37860</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>38856</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>39852</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>40848</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>7.7270000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.067</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.332000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.306999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28.762</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34.356999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.260999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44.976999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>55.466000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59.314</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>56.005000000000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64.036000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>74.108999999999995</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>84.588999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>95.375</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>82.677000000000007</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>94.099000000000004</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>95.99</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>108.997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>108.983</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100.89100000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>126.06399999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>127.307</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>119.706</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>169.11600000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>170.82900000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>149.339</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>166.50299999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>143.91399999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>175.71899999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>171.566</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>176.35</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>168.739</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>172.15700000000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>208.23500000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>166.077</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>169.685</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MultiThreaded</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>4992</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5988</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6984</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7980</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8976</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9972</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10968</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11964</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12960</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13956</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14952</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15948</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16944</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17940</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18936</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19932</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20928</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21924</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22920</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23916</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>24912</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25908</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>26904</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>27900</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>28896</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>29892</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>30888</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>31884</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>32880</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>33876</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>34872</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>35868</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>36864</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>37860</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>38856</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>39852</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>40848</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>7.3860000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.426</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.8030000000000008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.938000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.446</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.506</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.903</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.093</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.236999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19.084</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25.445</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26.146000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32.018999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>34.676000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>33.668999999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>38.652999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>35.274999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41.232999999999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43.959000000000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43.460999999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>38.78</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44.999000000000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>51.148000000000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>51.424999999999997</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>50.473999999999997</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>54.045000000000002</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>56.201000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="419976456"/>
+        <c:axId val="419974888"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="419976456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Connections</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="419974888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="419974888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>RTT (S)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="419976456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>157163</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -359,7 +2142,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,5 +2659,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added some Graphable data
</commit_message>
<xml_diff>
--- a/Logfiles/AverageRTT_512.xlsx
+++ b/Logfiles/AverageRTT_512.xlsx
@@ -1843,16 +1843,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>157163</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>